<commit_message>
Locale creation bug fixes
</commit_message>
<xml_diff>
--- a/public/Example_Template.xlsx
+++ b/public/Example_Template.xlsx
@@ -8,22 +8,23 @@
     <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Example_data" sheetId="1" r:id="rId4"/>
+    <sheet name="Explanation" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1645282330" val="1042" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1645282330" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1645282330" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1645282330"/>
+      <pm:revision xmlns:pm="smNativeData" day="1646179446" val="1042" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1646179446" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1646179446" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1646179446"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="304">
   <si>
     <t>Title</t>
   </si>
@@ -43,9 +44,6 @@
     <t>mpId</t>
   </si>
   <si>
-    <t>apiId</t>
-  </si>
-  <si>
     <t>Argan Oil &amp; Aloe Vera Sulfate-Free Shampoo</t>
   </si>
   <si>
@@ -929,6 +927,132 @@
   </si>
   <si>
     <t>'381519019739</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="0"/>
+        <family val="2"/>
+        <sz val="10"/>
+        <b/>
+        <i val="0"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:charSpec xmlns:pm="smNativeData" id="1646179446">
+              <pm:latin face="Arial" sz="200" weight="bold" i="0"/>
+              <pm:cs/>
+              <pm:ea/>
+            </pm:charSpec>
+          </ext>
+        </extLst>
+      </rPr>
+      <t xml:space="preserve">url </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="0"/>
+        <family val="2"/>
+        <sz val="10"/>
+        <b val="0"/>
+        <i val="0"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:charSpec xmlns:pm="smNativeData" id="1646179446">
+              <pm:latin face="Arial" sz="200" weight="normal" i="0"/>
+              <pm:cs/>
+              <pm:ea/>
+            </pm:charSpec>
+          </ext>
+        </extLst>
+      </rPr>
+      <t>is mandatory field for all types of pages.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="0"/>
+        <family val="2"/>
+        <sz val="10"/>
+        <b/>
+        <i val="0"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:charSpec xmlns:pm="smNativeData" id="1646179446">
+              <pm:latin face="Arial" sz="200" weight="bold" i="0"/>
+              <pm:cs/>
+              <pm:ea/>
+            </pm:charSpec>
+          </ext>
+        </extLst>
+      </rPr>
+      <t xml:space="preserve">SKU </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="0"/>
+        <family val="2"/>
+        <sz val="10"/>
+        <b val="0"/>
+        <i val="0"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:charSpec xmlns:pm="smNativeData" id="1646179446">
+              <pm:latin face="Arial" sz="200" weight="normal" i="0"/>
+              <pm:cs/>
+              <pm:ea/>
+            </pm:charSpec>
+          </ext>
+        </extLst>
+      </rPr>
+      <t>is mandatory for pages of type "product". If actual SKU value is not known, assing a random value that is unique between the product pages. Ascending numbers from 1 to ... is ok.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="0"/>
+        <family val="2"/>
+        <sz val="10"/>
+        <b/>
+        <i val="0"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:charSpec xmlns:pm="smNativeData" id="1646179446">
+              <pm:latin face="Arial" sz="200" weight="bold" i="0"/>
+              <pm:cs/>
+              <pm:ea/>
+            </pm:charSpec>
+          </ext>
+        </extLst>
+      </rPr>
+      <t>Type "product"</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="0"/>
+        <family val="2"/>
+        <sz val="10"/>
+        <b val="0"/>
+        <i val="0"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:charSpec xmlns:pm="smNativeData" id="1646179446">
+              <pm:latin face="Arial" sz="200" weight="normal" i="0"/>
+              <pm:cs/>
+              <pm:ea/>
+            </pm:charSpec>
+          </ext>
+        </extLst>
+      </rPr>
+      <t xml:space="preserve"> is mandatory for product pages. Rest of the page types can be entered at will.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -945,7 +1069,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
   </numFmts>
-  <fonts count="101">
+  <fonts count="104">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -953,7 +1077,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -968,7 +1092,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -983,23 +1107,23 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="none" kern="1">
-            <pm:latin face="Calibri" sz="220" lang="default"/>
-            <pm:cs face="Basic Roman" sz="220" lang="default"/>
-            <pm:ea face="Basic Roman" sz="220" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="none" kern="1">
+            <pm:latin face="Calibri" sz="220" lang="default"/>
+            <pm:cs face="Basic Roman" sz="220" lang="default"/>
+            <pm:ea face="Basic Roman" sz="220" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1016,7 +1140,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1033,7 +1157,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1050,7 +1174,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1067,7 +1191,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1084,7 +1208,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1101,7 +1225,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1118,7 +1242,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1135,7 +1259,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1152,7 +1276,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1169,7 +1293,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1186,7 +1310,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1203,7 +1327,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1220,7 +1344,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1237,7 +1361,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1254,7 +1378,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1271,7 +1395,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1288,7 +1412,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1305,7 +1429,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1322,7 +1446,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1339,7 +1463,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1356,7 +1480,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1373,7 +1497,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1390,7 +1514,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1407,7 +1531,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1424,7 +1548,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1441,7 +1565,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1458,7 +1582,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1475,7 +1599,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1492,7 +1616,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1509,7 +1633,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1526,7 +1650,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1543,7 +1667,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1560,7 +1684,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1577,7 +1701,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1594,7 +1718,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1611,7 +1735,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1628,7 +1752,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1645,7 +1769,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1662,7 +1786,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1679,7 +1803,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1696,7 +1820,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1713,7 +1837,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1730,7 +1854,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1747,7 +1871,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1764,7 +1888,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1781,7 +1905,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1798,7 +1922,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1815,7 +1939,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1832,7 +1956,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1849,7 +1973,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1866,7 +1990,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1883,7 +2007,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1900,7 +2024,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1917,7 +2041,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1934,7 +2058,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1951,7 +2075,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1968,7 +2092,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1985,7 +2109,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2002,7 +2126,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2019,7 +2143,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2036,7 +2160,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2053,7 +2177,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2070,7 +2194,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2087,7 +2211,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2104,7 +2228,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2121,7 +2245,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2138,7 +2262,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2155,7 +2279,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2172,7 +2296,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2189,7 +2313,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2206,7 +2330,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2223,7 +2347,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2240,7 +2364,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2257,7 +2381,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2274,7 +2398,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2291,7 +2415,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2308,7 +2432,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2325,7 +2449,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2342,7 +2466,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2359,7 +2483,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2376,7 +2500,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2393,7 +2517,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2410,7 +2534,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2427,7 +2551,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2444,7 +2568,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2461,7 +2585,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2478,7 +2602,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2495,7 +2619,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2512,7 +2636,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2529,7 +2653,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2546,7 +2670,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2563,7 +2687,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2580,7 +2704,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2597,7 +2721,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2614,7 +2738,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2631,7 +2755,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2648,11 +2772,59 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645282330" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
             <hyperlink type="6" url="https://herbalessences.com/en-us/our-products/set-me-up/set-me-up-hairspray/" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="none" kern="1">
+            <pm:latin face="Calibri" sz="220" lang="default"/>
+            <pm:cs face="Basic Roman" sz="220" lang="default"/>
+            <pm:ea face="Basic Roman" sz="220" lang="default"/>
+            <hyperlink type="6" url="https://herbalessences.com/en-us/our-products/argan-oil/argan-oil-aloe-sulfate-hair-shampoo/" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="none" kern="1">
+            <pm:latin face="Calibri" sz="220" lang="default"/>
+            <pm:cs face="Basic Roman" sz="220" lang="default"/>
+            <pm:ea face="Basic Roman" sz="220" lang="default"/>
+            <hyperlink type="6" url="https://herbalessences.com/en-us/our-products/argan-oil/argan-oil-aloe-sulfate-hair-conditioner/" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646179446" ulstyle="none" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -2671,7 +2843,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1645282330" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1646179446" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -2693,7 +2865,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1645282330"/>
+          <pm:border xmlns:pm="smNativeData" id="1646179446"/>
         </ext>
       </extLst>
     </border>
@@ -2712,7 +2884,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1645282330"/>
+          <pm:border xmlns:pm="smNativeData" id="1646179446"/>
         </ext>
       </extLst>
     </border>
@@ -2720,7 +2892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3023,6 +3195,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -3032,7 +3210,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1645282330" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1646179446" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -3302,7 +3480,7 @@
   <dimension ref="A1:G99"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="13" defaultColWidth="14.432432" defaultRowHeight="15.75" customHeight="1"/>
@@ -3336,23 +3514,23 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="102" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>779532</v>
@@ -3361,17 +3539,19 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="103" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>779531</v>
@@ -3380,17 +3560,19 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="102" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>462741</v>
@@ -3399,17 +3581,19 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="103" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>462742</v>
@@ -3418,17 +3602,19 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="102" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>462732</v>
@@ -3437,17 +3623,19 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="C7" s="103" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>462734</v>
@@ -3456,17 +3644,19 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="102" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>1032330</v>
@@ -3475,17 +3665,19 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="103" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>462738</v>
@@ -3494,17 +3686,19 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="C10" s="102" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>462739</v>
@@ -3513,17 +3707,19 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="C11" s="103" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>462740</v>
@@ -3532,17 +3728,19 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="C12" s="102" t="n">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>462730</v>
@@ -3551,17 +3749,19 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="C13" s="103" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>462743</v>
@@ -3570,17 +3770,19 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="C14" s="102" t="n">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>462708</v>
@@ -3589,17 +3791,19 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="C15" s="103" t="n">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>794194</v>
@@ -3608,17 +3812,19 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="C16" s="102" t="n">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>794188</v>
@@ -3627,17 +3833,19 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="C17" s="103" t="n">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>776662</v>
@@ -3646,17 +3854,19 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="C18" s="102" t="n">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>794186</v>
@@ -3665,17 +3875,19 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="C19" s="103" t="n">
+        <v>18</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>865025</v>
@@ -3684,17 +3896,19 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="C20" s="102" t="n">
+        <v>19</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>389135</v>
@@ -3703,17 +3917,19 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="C21" s="103" t="n">
+        <v>20</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>389123</v>
@@ -3722,17 +3938,19 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="C22" s="102" t="n">
+        <v>21</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>462744</v>
@@ -3741,17 +3959,19 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="C23" s="103" t="n">
+        <v>22</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" s="2" t="n">
         <v>462745</v>
@@ -3760,17 +3980,19 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="C24" s="102" t="n">
+        <v>23</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" s="2" t="n">
         <v>865017</v>
@@ -3779,17 +4001,19 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="C25" s="103" t="n">
+        <v>24</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" s="2" t="n">
         <v>776663</v>
@@ -3798,17 +4022,19 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="C26" s="102" t="n">
+        <v>25</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" s="2" t="n">
         <v>462729</v>
@@ -3817,17 +4043,19 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="C27" s="103" t="n">
+        <v>26</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="29"/>
-      <c r="D27" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="E27" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27" s="2" t="n">
         <v>462727</v>
@@ -3836,17 +4064,19 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="C28" s="102" t="n">
+        <v>27</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" s="2" t="n">
         <v>389101</v>
@@ -3855,17 +4085,19 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="C29" s="103" t="n">
+        <v>28</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" s="2" t="n">
         <v>389092</v>
@@ -3874,17 +4106,19 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="C30" s="102" t="n">
+        <v>29</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" s="2" t="n">
         <v>462724</v>
@@ -3893,17 +4127,19 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="33" t="s">
+      <c r="C31" s="103" t="n">
+        <v>30</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="E31" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" s="2" t="n">
         <v>462719</v>
@@ -3912,17 +4148,19 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="C32" s="102" t="n">
+        <v>31</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="34"/>
-      <c r="D32" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="E32" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" s="2" t="n">
         <v>434024</v>
@@ -3931,17 +4169,19 @@
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="C33" s="103" t="n">
+        <v>32</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="35"/>
-      <c r="D33" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" s="2" t="n">
         <v>776664</v>
@@ -3950,17 +4190,19 @@
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="36" t="s">
+      <c r="C34" s="102" t="n">
+        <v>33</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="E34" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" s="2" t="n">
         <v>462728</v>
@@ -3969,17 +4211,19 @@
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="37" t="s">
+      <c r="C35" s="103" t="n">
+        <v>34</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="37"/>
-      <c r="D35" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" s="2" t="n">
         <v>389073</v>
@@ -3988,17 +4232,19 @@
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="38" t="s">
+      <c r="C36" s="102" t="n">
+        <v>35</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C36" s="38"/>
-      <c r="D36" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="E36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36" s="2" t="n">
         <v>389065</v>
@@ -4007,17 +4253,19 @@
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1">
       <c r="A37" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="B37" s="39" t="s">
+      <c r="C37" s="103" t="n">
+        <v>36</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C37" s="39"/>
-      <c r="D37" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="E37" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" s="2" t="n">
         <v>1023721</v>
@@ -4026,17 +4274,19 @@
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="C38" s="102" t="n">
+        <v>37</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C38" s="40"/>
-      <c r="D38" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="E38" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" s="2" t="n">
         <v>776643</v>
@@ -4045,17 +4295,19 @@
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="B39" s="41" t="s">
+      <c r="C39" s="103" t="n">
+        <v>38</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C39" s="41"/>
-      <c r="D39" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="E39" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" s="2" t="n">
         <v>395908</v>
@@ -4064,17 +4316,19 @@
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1">
       <c r="A40" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="C40" s="102" t="n">
+        <v>39</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C40" s="42"/>
-      <c r="D40" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="E40" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F40" s="2" t="n">
         <v>389038</v>
@@ -4083,17 +4337,19 @@
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="43" t="s">
+      <c r="C41" s="103" t="n">
+        <v>40</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C41" s="43"/>
-      <c r="D41" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="E41" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F41" s="2" t="n">
         <v>389086</v>
@@ -4102,17 +4358,19 @@
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1">
       <c r="A42" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="44" t="s">
+      <c r="C42" s="102" t="n">
+        <v>41</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C42" s="44"/>
-      <c r="D42" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="E42" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" s="2" t="n">
         <v>389081</v>
@@ -4121,17 +4379,19 @@
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B43" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="B43" s="45" t="s">
+      <c r="C43" s="103" t="n">
+        <v>42</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C43" s="45"/>
-      <c r="D43" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="E43" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" s="2" t="n">
         <v>462715</v>
@@ -4140,17 +4400,19 @@
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1">
       <c r="A44" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="B44" s="46" t="s">
+      <c r="C44" s="102" t="n">
+        <v>43</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C44" s="46"/>
-      <c r="D44" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="E44" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44" s="2" t="n">
         <v>462691</v>
@@ -4159,17 +4421,19 @@
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1">
       <c r="A45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="B45" s="47" t="s">
+      <c r="C45" s="103" t="n">
+        <v>44</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C45" s="47"/>
-      <c r="D45" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="E45" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" s="2" t="n">
         <v>462671</v>
@@ -4178,17 +4442,19 @@
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1">
       <c r="A46" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="B46" s="48" t="s">
+      <c r="C46" s="102" t="n">
+        <v>45</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C46" s="48"/>
-      <c r="D46" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="E46" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F46" s="2" t="n">
         <v>389119</v>
@@ -4197,17 +4463,19 @@
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1">
       <c r="A47" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="B47" s="49" t="s">
+      <c r="C47" s="103" t="n">
+        <v>46</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C47" s="49"/>
-      <c r="D47" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="E47" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" s="2" t="n">
         <v>389108</v>
@@ -4216,17 +4484,19 @@
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1">
       <c r="A48" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B48" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="B48" s="50" t="s">
+      <c r="C48" s="102" t="n">
+        <v>47</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C48" s="50"/>
-      <c r="D48" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="E48" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F48" s="2" t="n">
         <v>776650</v>
@@ -4235,17 +4505,19 @@
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1">
       <c r="A49" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B49" s="51" t="s">
         <v>149</v>
       </c>
-      <c r="B49" s="51" t="s">
+      <c r="C49" s="103" t="n">
+        <v>48</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C49" s="51"/>
-      <c r="D49" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="E49" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F49" s="2" t="n">
         <v>389030</v>
@@ -4254,17 +4526,19 @@
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1">
       <c r="A50" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B50" s="52" t="s">
         <v>152</v>
       </c>
-      <c r="B50" s="52" t="s">
+      <c r="C50" s="102" t="n">
+        <v>49</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C50" s="52"/>
-      <c r="D50" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="E50" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" s="2" t="n">
         <v>389023</v>
@@ -4273,17 +4547,19 @@
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1">
       <c r="A51" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B51" s="53" t="s">
         <v>155</v>
       </c>
-      <c r="B51" s="53" t="s">
+      <c r="C51" s="103" t="n">
+        <v>50</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C51" s="53"/>
-      <c r="D51" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="E51" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" s="2" t="n">
         <v>389048</v>
@@ -4292,17 +4568,19 @@
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1">
       <c r="A52" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B52" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="B52" s="54" t="s">
+      <c r="C52" s="102" t="n">
+        <v>51</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C52" s="54"/>
-      <c r="D52" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="E52" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" s="2" t="n">
         <v>389062</v>
@@ -4311,17 +4589,19 @@
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1">
       <c r="A53" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B53" s="55" t="s">
         <v>161</v>
       </c>
-      <c r="B53" s="55" t="s">
+      <c r="C53" s="103" t="n">
+        <v>52</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C53" s="55"/>
-      <c r="D53" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="E53" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" s="2" t="n">
         <v>389059</v>
@@ -4330,17 +4610,19 @@
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1">
       <c r="A54" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B54" s="56" t="s">
         <v>164</v>
       </c>
-      <c r="B54" s="56" t="s">
+      <c r="C54" s="102" t="n">
+        <v>53</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C54" s="56"/>
-      <c r="D54" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="E54" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" s="2" t="n">
         <v>462704</v>
@@ -4349,17 +4631,19 @@
     </row>
     <row r="55" spans="1:7" ht="15.75" customHeight="1">
       <c r="A55" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B55" s="57" t="s">
         <v>167</v>
       </c>
-      <c r="B55" s="57" t="s">
+      <c r="C55" s="103" t="n">
+        <v>54</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C55" s="57"/>
-      <c r="D55" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="E55" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" s="2" t="n">
         <v>462677</v>
@@ -4368,17 +4652,19 @@
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1">
       <c r="A56" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B56" s="58" t="s">
         <v>170</v>
       </c>
-      <c r="B56" s="58" t="s">
+      <c r="C56" s="102" t="n">
+        <v>55</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C56" s="58"/>
-      <c r="D56" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="E56" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" s="2" t="n">
         <v>462721</v>
@@ -4387,17 +4673,19 @@
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1">
       <c r="A57" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B57" s="59" t="s">
         <v>173</v>
       </c>
-      <c r="B57" s="59" t="s">
+      <c r="C57" s="103" t="n">
+        <v>56</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C57" s="59"/>
-      <c r="D57" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="E57" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" s="2" t="n">
         <v>462720</v>
@@ -4406,17 +4694,19 @@
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1">
       <c r="A58" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B58" s="60" t="s">
         <v>176</v>
       </c>
-      <c r="B58" s="60" t="s">
+      <c r="C58" s="102" t="n">
+        <v>57</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C58" s="60"/>
-      <c r="D58" s="2" t="s">
-        <v>178</v>
-      </c>
       <c r="E58" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" s="2" t="n">
         <v>462711</v>
@@ -4425,17 +4715,19 @@
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1">
       <c r="A59" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B59" s="61" t="s">
         <v>179</v>
       </c>
-      <c r="B59" s="61" t="s">
+      <c r="C59" s="102" t="n">
+        <v>58</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C59" s="61"/>
-      <c r="D59" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="E59" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" s="2" t="n">
         <v>462696</v>
@@ -4444,17 +4736,19 @@
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1">
       <c r="A60" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B60" s="62" t="s">
         <v>182</v>
       </c>
-      <c r="B60" s="62" t="s">
+      <c r="C60" s="103" t="n">
+        <v>59</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C60" s="62"/>
-      <c r="D60" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="E60" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" s="2" t="n">
         <v>462700</v>
@@ -4463,17 +4757,19 @@
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1">
       <c r="A61" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B61" s="63" t="s">
         <v>185</v>
       </c>
-      <c r="B61" s="63" t="s">
+      <c r="C61" s="102" t="n">
+        <v>60</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C61" s="63"/>
-      <c r="D61" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="E61" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F61" s="2" t="n">
         <v>389012</v>
@@ -4482,17 +4778,19 @@
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1">
       <c r="A62" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B62" s="64" t="s">
         <v>188</v>
       </c>
-      <c r="B62" s="64" t="s">
+      <c r="C62" s="103" t="n">
+        <v>61</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C62" s="64"/>
-      <c r="D62" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="E62" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" s="2" t="n">
         <v>389051</v>
@@ -4501,17 +4799,19 @@
     </row>
     <row r="63" spans="1:7" ht="15.75" customHeight="1">
       <c r="A63" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B63" s="65" t="s">
         <v>191</v>
       </c>
-      <c r="B63" s="65" t="s">
+      <c r="C63" s="102" t="n">
+        <v>62</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C63" s="65"/>
-      <c r="D63" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="E63" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" s="2" t="n">
         <v>1023722</v>
@@ -4520,17 +4820,19 @@
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1">
       <c r="A64" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B64" s="66" t="s">
         <v>194</v>
       </c>
-      <c r="B64" s="66" t="s">
+      <c r="C64" s="103" t="n">
+        <v>63</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C64" s="66"/>
-      <c r="D64" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="E64" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" s="2" t="n">
         <v>794169</v>
@@ -4539,17 +4841,19 @@
     </row>
     <row r="65" spans="1:7" ht="15.75" customHeight="1">
       <c r="A65" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B65" s="67" t="s">
         <v>197</v>
       </c>
-      <c r="B65" s="67" t="s">
+      <c r="C65" s="102" t="n">
+        <v>64</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C65" s="67"/>
-      <c r="D65" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="E65" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" s="2" t="n">
         <v>462736</v>
@@ -4558,17 +4862,19 @@
     </row>
     <row r="66" spans="1:7" ht="15.75" customHeight="1">
       <c r="A66" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B66" s="68" t="s">
         <v>200</v>
       </c>
-      <c r="B66" s="68" t="s">
+      <c r="C66" s="103" t="n">
+        <v>65</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C66" s="68"/>
-      <c r="D66" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="E66" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" s="2" t="n">
         <v>794198</v>
@@ -4577,17 +4883,19 @@
     </row>
     <row r="67" spans="1:7" ht="15.75" customHeight="1">
       <c r="A67" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B67" s="69" t="s">
         <v>203</v>
       </c>
-      <c r="B67" s="69" t="s">
+      <c r="C67" s="102" t="n">
+        <v>66</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C67" s="69"/>
-      <c r="D67" s="2" t="s">
-        <v>205</v>
-      </c>
       <c r="E67" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" s="2" t="n">
         <v>794190</v>
@@ -4596,17 +4904,19 @@
     </row>
     <row r="68" spans="1:7" ht="15.75" customHeight="1">
       <c r="A68" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B68" s="70" t="s">
         <v>206</v>
       </c>
-      <c r="B68" s="70" t="s">
+      <c r="C68" s="103" t="n">
+        <v>67</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C68" s="70"/>
-      <c r="D68" s="2" t="s">
-        <v>208</v>
-      </c>
       <c r="E68" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" s="2" t="n">
         <v>865027</v>
@@ -4615,17 +4925,19 @@
     </row>
     <row r="69" spans="1:7" ht="15.75" customHeight="1">
       <c r="A69" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B69" s="71" t="s">
         <v>209</v>
       </c>
-      <c r="B69" s="71" t="s">
+      <c r="C69" s="102" t="n">
+        <v>68</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C69" s="71"/>
-      <c r="D69" s="2" t="s">
-        <v>211</v>
-      </c>
       <c r="E69" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" s="2" t="n">
         <v>865028</v>
@@ -4634,17 +4946,19 @@
     </row>
     <row r="70" spans="1:7" ht="15.75" customHeight="1">
       <c r="A70" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B70" s="72" t="s">
         <v>212</v>
       </c>
-      <c r="B70" s="72" t="s">
+      <c r="C70" s="103" t="n">
+        <v>69</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C70" s="72"/>
-      <c r="D70" s="2" t="s">
-        <v>214</v>
-      </c>
       <c r="E70" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" s="2" t="n">
         <v>462757</v>
@@ -4653,17 +4967,19 @@
     </row>
     <row r="71" spans="1:7" ht="15.75" customHeight="1">
       <c r="A71" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B71" s="73" t="s">
         <v>215</v>
       </c>
-      <c r="B71" s="73" t="s">
+      <c r="C71" s="102" t="n">
+        <v>70</v>
+      </c>
+      <c r="D71" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C71" s="73"/>
-      <c r="D71" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="E71" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" s="2" t="n">
         <v>467893</v>
@@ -4672,17 +4988,19 @@
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1">
       <c r="A72" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B72" s="74" t="s">
         <v>218</v>
       </c>
-      <c r="B72" s="74" t="s">
+      <c r="C72" s="103" t="n">
+        <v>71</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C72" s="74"/>
-      <c r="D72" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="E72" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" s="2" t="n">
         <v>462803</v>
@@ -4691,17 +5009,19 @@
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1">
       <c r="A73" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B73" s="75" t="s">
         <v>221</v>
       </c>
-      <c r="B73" s="75" t="s">
+      <c r="C73" s="102" t="n">
+        <v>72</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C73" s="75"/>
-      <c r="D73" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="E73" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" s="2" t="n">
         <v>462758</v>
@@ -4710,17 +5030,19 @@
     </row>
     <row r="74" spans="1:7" ht="15.75" customHeight="1">
       <c r="A74" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B74" s="76" t="s">
         <v>224</v>
       </c>
-      <c r="B74" s="76" t="s">
+      <c r="C74" s="103" t="n">
+        <v>73</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C74" s="76"/>
-      <c r="D74" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="E74" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" s="2" t="n">
         <v>462810</v>
@@ -4729,17 +5051,19 @@
     </row>
     <row r="75" spans="1:7" ht="15.75" customHeight="1">
       <c r="A75" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B75" s="77" t="s">
         <v>227</v>
       </c>
-      <c r="B75" s="77" t="s">
+      <c r="C75" s="102" t="n">
+        <v>74</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C75" s="77"/>
-      <c r="D75" s="2" t="s">
-        <v>229</v>
-      </c>
       <c r="E75" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" s="2" t="n">
         <v>462819</v>
@@ -4748,17 +5072,19 @@
     </row>
     <row r="76" spans="1:7" ht="15.75" customHeight="1">
       <c r="A76" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B76" s="78" t="s">
         <v>230</v>
       </c>
-      <c r="B76" s="78" t="s">
+      <c r="C76" s="103" t="n">
+        <v>75</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C76" s="78"/>
-      <c r="D76" s="2" t="s">
-        <v>232</v>
-      </c>
       <c r="E76" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" s="2" t="n">
         <v>462833</v>
@@ -4767,17 +5093,19 @@
     </row>
     <row r="77" spans="1:7" ht="15.75" customHeight="1">
       <c r="A77" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B77" s="79" t="s">
         <v>233</v>
       </c>
-      <c r="B77" s="79" t="s">
+      <c r="C77" s="102" t="n">
+        <v>76</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C77" s="79"/>
-      <c r="D77" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="E77" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" s="2" t="n">
         <v>462685</v>
@@ -4786,17 +5114,19 @@
     </row>
     <row r="78" spans="1:7" ht="15.75" customHeight="1">
       <c r="A78" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B78" s="80" t="s">
         <v>236</v>
       </c>
-      <c r="B78" s="80" t="s">
+      <c r="C78" s="103" t="n">
+        <v>77</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C78" s="80"/>
-      <c r="D78" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="E78" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" s="2" t="n">
         <v>776608</v>
@@ -4805,17 +5135,19 @@
     </row>
     <row r="79" spans="1:7" ht="15.75" customHeight="1">
       <c r="A79" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B79" s="81" t="s">
         <v>239</v>
       </c>
-      <c r="B79" s="81" t="s">
+      <c r="C79" s="102" t="n">
+        <v>78</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C79" s="81"/>
-      <c r="D79" s="2" t="s">
-        <v>241</v>
-      </c>
       <c r="E79" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" s="2" t="n">
         <v>776618</v>
@@ -4824,17 +5156,19 @@
     </row>
     <row r="80" spans="1:7" ht="15.75" customHeight="1">
       <c r="A80" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B80" s="82" t="s">
         <v>242</v>
       </c>
-      <c r="B80" s="82" t="s">
+      <c r="C80" s="102" t="n">
+        <v>79</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C80" s="82"/>
-      <c r="D80" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="E80" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" s="2" t="n">
         <v>776633</v>
@@ -4843,17 +5177,19 @@
     </row>
     <row r="81" spans="1:7" ht="15.75" customHeight="1">
       <c r="A81" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B81" s="83" t="s">
         <v>245</v>
       </c>
-      <c r="B81" s="83" t="s">
+      <c r="C81" s="103" t="n">
+        <v>80</v>
+      </c>
+      <c r="D81" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C81" s="83"/>
-      <c r="D81" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="E81" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" s="2" t="n">
         <v>794183</v>
@@ -4862,17 +5198,19 @@
     </row>
     <row r="82" spans="1:7" ht="15.75" customHeight="1">
       <c r="A82" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B82" s="84" t="s">
         <v>248</v>
       </c>
-      <c r="B82" s="84" t="s">
+      <c r="C82" s="102" t="n">
+        <v>81</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C82" s="84"/>
-      <c r="D82" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="E82" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" s="2" t="n">
         <v>794182</v>
@@ -4881,17 +5219,19 @@
     </row>
     <row r="83" spans="1:7" ht="15.75" customHeight="1">
       <c r="A83" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B83" s="85" t="s">
         <v>251</v>
       </c>
-      <c r="B83" s="85" t="s">
+      <c r="C83" s="103" t="n">
+        <v>82</v>
+      </c>
+      <c r="D83" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C83" s="85"/>
-      <c r="D83" s="2" t="s">
-        <v>253</v>
-      </c>
       <c r="E83" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" s="2" t="n">
         <v>776626</v>
@@ -4900,17 +5240,19 @@
     </row>
     <row r="84" spans="1:7" ht="15.75" customHeight="1">
       <c r="A84" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B84" s="86" t="s">
         <v>254</v>
       </c>
-      <c r="B84" s="86" t="s">
+      <c r="C84" s="102" t="n">
+        <v>83</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C84" s="86"/>
-      <c r="D84" s="2" t="s">
-        <v>256</v>
-      </c>
       <c r="E84" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" s="2" t="n">
         <v>776665</v>
@@ -4919,17 +5261,19 @@
     </row>
     <row r="85" spans="1:7" ht="15.75" customHeight="1">
       <c r="A85" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B85" s="87" t="s">
         <v>257</v>
       </c>
-      <c r="B85" s="87" t="s">
+      <c r="C85" s="103" t="n">
+        <v>84</v>
+      </c>
+      <c r="D85" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C85" s="87"/>
-      <c r="D85" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="E85" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" s="2" t="n">
         <v>389431</v>
@@ -4938,17 +5282,19 @@
     </row>
     <row r="86" spans="1:7" ht="15.75" customHeight="1">
       <c r="A86" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B86" s="88" t="s">
         <v>260</v>
       </c>
-      <c r="B86" s="88" t="s">
+      <c r="C86" s="102" t="n">
+        <v>85</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C86" s="88"/>
-      <c r="D86" s="2" t="s">
-        <v>262</v>
-      </c>
       <c r="E86" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" s="2" t="n">
         <v>776606</v>
@@ -4957,17 +5303,19 @@
     </row>
     <row r="87" spans="1:7" ht="15.75" customHeight="1">
       <c r="A87" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B87" s="89" t="s">
         <v>263</v>
       </c>
-      <c r="B87" s="89" t="s">
+      <c r="C87" s="103" t="n">
+        <v>86</v>
+      </c>
+      <c r="D87" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C87" s="89"/>
-      <c r="D87" s="2" t="s">
-        <v>265</v>
-      </c>
       <c r="E87" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F87" s="2" t="n">
         <v>776590</v>
@@ -4976,17 +5324,19 @@
     </row>
     <row r="88" spans="1:7" ht="15.75" customHeight="1">
       <c r="A88" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B88" s="90" t="s">
         <v>266</v>
       </c>
-      <c r="B88" s="90" t="s">
+      <c r="C88" s="102" t="n">
+        <v>87</v>
+      </c>
+      <c r="D88" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C88" s="90"/>
-      <c r="D88" s="2" t="s">
-        <v>268</v>
-      </c>
       <c r="E88" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F88" s="2" t="n">
         <v>776669</v>
@@ -4995,17 +5345,19 @@
     </row>
     <row r="89" spans="1:7" ht="15.75" customHeight="1">
       <c r="A89" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B89" s="91" t="s">
         <v>269</v>
       </c>
-      <c r="B89" s="91" t="s">
+      <c r="C89" s="103" t="n">
+        <v>88</v>
+      </c>
+      <c r="D89" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C89" s="91"/>
-      <c r="D89" s="2" t="s">
-        <v>271</v>
-      </c>
       <c r="E89" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F89" s="2" t="n">
         <v>776644</v>
@@ -5014,17 +5366,19 @@
     </row>
     <row r="90" spans="1:7" ht="15.75" customHeight="1">
       <c r="A90" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B90" s="92" t="s">
         <v>272</v>
       </c>
-      <c r="B90" s="92" t="s">
+      <c r="C90" s="102" t="n">
+        <v>89</v>
+      </c>
+      <c r="D90" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C90" s="92"/>
-      <c r="D90" s="2" t="s">
-        <v>274</v>
-      </c>
       <c r="E90" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F90" s="2" t="n">
         <v>389423</v>
@@ -5033,17 +5387,19 @@
     </row>
     <row r="91" spans="1:7" ht="15.75" customHeight="1">
       <c r="A91" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B91" s="93" t="s">
         <v>275</v>
       </c>
-      <c r="B91" s="93" t="s">
+      <c r="C91" s="103" t="n">
+        <v>90</v>
+      </c>
+      <c r="D91" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C91" s="93"/>
-      <c r="D91" s="2" t="s">
-        <v>277</v>
-      </c>
       <c r="E91" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" s="2" t="n">
         <v>776592</v>
@@ -5052,17 +5408,19 @@
     </row>
     <row r="92" spans="1:7" ht="15.75" customHeight="1">
       <c r="A92" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B92" s="94" t="s">
         <v>278</v>
       </c>
-      <c r="B92" s="94" t="s">
+      <c r="C92" s="102" t="n">
+        <v>91</v>
+      </c>
+      <c r="D92" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C92" s="94"/>
-      <c r="D92" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="E92" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F92" s="2" t="n">
         <v>776671</v>
@@ -5071,17 +5429,19 @@
     </row>
     <row r="93" spans="1:7" ht="15.75" customHeight="1">
       <c r="A93" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B93" s="95" t="s">
         <v>281</v>
       </c>
-      <c r="B93" s="95" t="s">
+      <c r="C93" s="103" t="n">
+        <v>92</v>
+      </c>
+      <c r="D93" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C93" s="95"/>
-      <c r="D93" s="2" t="s">
-        <v>283</v>
-      </c>
       <c r="E93" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" s="2" t="n">
         <v>776670</v>
@@ -5090,17 +5450,19 @@
     </row>
     <row r="94" spans="1:7" ht="15.75" customHeight="1">
       <c r="A94" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B94" s="96" t="s">
         <v>284</v>
       </c>
-      <c r="B94" s="96" t="s">
+      <c r="C94" s="102" t="n">
+        <v>93</v>
+      </c>
+      <c r="D94" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="C94" s="96"/>
-      <c r="D94" s="2" t="s">
-        <v>286</v>
-      </c>
       <c r="E94" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F94" s="2" t="n">
         <v>794202</v>
@@ -5109,17 +5471,19 @@
     </row>
     <row r="95" spans="1:7" ht="15.75" customHeight="1">
       <c r="A95" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B95" s="97" t="s">
         <v>287</v>
       </c>
-      <c r="B95" s="97" t="s">
+      <c r="C95" s="102" t="n">
+        <v>94</v>
+      </c>
+      <c r="D95" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C95" s="97"/>
-      <c r="D95" s="2" t="s">
-        <v>289</v>
-      </c>
       <c r="E95" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" s="2" t="n">
         <v>794201</v>
@@ -5128,17 +5492,19 @@
     </row>
     <row r="96" spans="1:7" ht="15.75" customHeight="1">
       <c r="A96" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B96" s="98" t="s">
         <v>290</v>
       </c>
-      <c r="B96" s="98" t="s">
+      <c r="C96" s="103" t="n">
+        <v>95</v>
+      </c>
+      <c r="D96" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C96" s="98"/>
-      <c r="D96" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="E96" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" s="2" t="n">
         <v>1023727</v>
@@ -5147,17 +5513,19 @@
     </row>
     <row r="97" spans="1:7" ht="15.75" customHeight="1">
       <c r="A97" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B97" s="99" t="s">
         <v>293</v>
       </c>
-      <c r="B97" s="99" t="s">
+      <c r="C97" s="102" t="n">
+        <v>96</v>
+      </c>
+      <c r="D97" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C97" s="99"/>
-      <c r="D97" s="2" t="s">
-        <v>295</v>
-      </c>
       <c r="E97" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" s="2" t="n">
         <v>794181</v>
@@ -5166,17 +5534,19 @@
     </row>
     <row r="98" spans="1:7" ht="15.75" customHeight="1">
       <c r="A98" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B98" s="100" t="s">
         <v>296</v>
       </c>
-      <c r="B98" s="100" t="s">
+      <c r="C98" s="103" t="n">
+        <v>97</v>
+      </c>
+      <c r="D98" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C98" s="100"/>
-      <c r="D98" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="E98" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" s="2" t="n">
         <v>794200</v>
@@ -5185,17 +5555,19 @@
     </row>
     <row r="99" spans="1:7" ht="15.75" customHeight="1">
       <c r="A99" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B99" s="101" t="s">
         <v>299</v>
       </c>
-      <c r="B99" s="101" t="s">
+      <c r="C99" s="102" t="n">
+        <v>98</v>
+      </c>
+      <c r="D99" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C99" s="101"/>
-      <c r="D99" s="2" t="s">
-        <v>301</v>
-      </c>
       <c r="E99" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" s="2" t="n">
         <v>794177</v>
@@ -5206,107 +5578,203 @@
   <hyperlinks>
     <hyperlink ref="B2:C2" r:id="rId1"/>
     <hyperlink ref="B3:C3" r:id="rId2"/>
-    <hyperlink ref="B4:C4" r:id="rId3"/>
-    <hyperlink ref="B5:C5" r:id="rId4"/>
-    <hyperlink ref="B6:C6" r:id="rId5"/>
-    <hyperlink ref="B7:C7" r:id="rId6"/>
-    <hyperlink ref="B8:C8" r:id="rId7"/>
-    <hyperlink ref="B9:C9" r:id="rId8"/>
-    <hyperlink ref="B10:C10" r:id="rId9"/>
-    <hyperlink ref="B11:C11" r:id="rId10"/>
-    <hyperlink ref="B12:C12" r:id="rId11"/>
-    <hyperlink ref="B13:C13" r:id="rId12"/>
-    <hyperlink ref="B14:C14" r:id="rId13"/>
-    <hyperlink ref="B15:C15" r:id="rId14"/>
-    <hyperlink ref="B16:C16" r:id="rId15"/>
-    <hyperlink ref="B17:C17" r:id="rId16"/>
-    <hyperlink ref="B18:C18" r:id="rId17"/>
-    <hyperlink ref="B19:C19" r:id="rId18"/>
-    <hyperlink ref="B20:C20" r:id="rId19"/>
-    <hyperlink ref="B21:C21" r:id="rId20"/>
-    <hyperlink ref="B22:C22" r:id="rId21"/>
-    <hyperlink ref="B23:C23" r:id="rId22"/>
-    <hyperlink ref="B24:C24" r:id="rId23"/>
-    <hyperlink ref="B25:C25" r:id="rId24"/>
-    <hyperlink ref="B26:C26" r:id="rId25"/>
-    <hyperlink ref="B27:C27" r:id="rId26"/>
-    <hyperlink ref="B28:C28" r:id="rId27"/>
-    <hyperlink ref="B29:C29" r:id="rId28"/>
-    <hyperlink ref="B30:C30" r:id="rId29"/>
-    <hyperlink ref="B31:C31" r:id="rId30"/>
-    <hyperlink ref="B32:C32" r:id="rId31"/>
-    <hyperlink ref="B33:C33" r:id="rId32"/>
-    <hyperlink ref="B34:C34" r:id="rId33"/>
-    <hyperlink ref="B35:C35" r:id="rId34"/>
-    <hyperlink ref="B36:C36" r:id="rId35"/>
-    <hyperlink ref="B37:C37" r:id="rId36"/>
-    <hyperlink ref="B38:C38" r:id="rId37"/>
-    <hyperlink ref="B39:C39" r:id="rId38"/>
-    <hyperlink ref="B40:C40" r:id="rId39"/>
-    <hyperlink ref="B41:C41" r:id="rId40"/>
-    <hyperlink ref="B42:C42" r:id="rId41"/>
-    <hyperlink ref="B43:C43" r:id="rId42"/>
-    <hyperlink ref="B44:C44" r:id="rId43"/>
-    <hyperlink ref="B45:C45" r:id="rId44"/>
-    <hyperlink ref="B46:C46" r:id="rId45"/>
-    <hyperlink ref="B47:C47" r:id="rId46"/>
-    <hyperlink ref="B48:C48" r:id="rId47"/>
-    <hyperlink ref="B49:C49" r:id="rId48"/>
-    <hyperlink ref="B50:C50" r:id="rId49"/>
-    <hyperlink ref="B51:C51" r:id="rId50"/>
-    <hyperlink ref="B52:C52" r:id="rId51"/>
-    <hyperlink ref="B53:C53" r:id="rId52"/>
-    <hyperlink ref="B54:C54" r:id="rId53"/>
-    <hyperlink ref="B55:C55" r:id="rId54"/>
-    <hyperlink ref="B56:C56" r:id="rId55"/>
-    <hyperlink ref="B57:C57" r:id="rId56"/>
-    <hyperlink ref="B58:C58" r:id="rId57"/>
-    <hyperlink ref="B59:C59" r:id="rId58"/>
-    <hyperlink ref="B60:C60" r:id="rId59"/>
-    <hyperlink ref="B61:C61" r:id="rId60"/>
-    <hyperlink ref="B62:C62" r:id="rId61"/>
-    <hyperlink ref="B63:C63" r:id="rId62"/>
-    <hyperlink ref="B64:C64" r:id="rId63"/>
-    <hyperlink ref="B65:C65" r:id="rId64"/>
-    <hyperlink ref="B66:C66" r:id="rId65"/>
-    <hyperlink ref="B67:C67" r:id="rId66"/>
-    <hyperlink ref="B68:C68" r:id="rId67"/>
-    <hyperlink ref="B69:C69" r:id="rId68"/>
-    <hyperlink ref="B70:C70" r:id="rId69"/>
-    <hyperlink ref="B71:C71" r:id="rId70"/>
-    <hyperlink ref="B72:C72" r:id="rId71"/>
-    <hyperlink ref="B73:C73" r:id="rId72"/>
-    <hyperlink ref="B74:C74" r:id="rId73"/>
-    <hyperlink ref="B75:C75" r:id="rId74"/>
-    <hyperlink ref="B76:C76" r:id="rId75"/>
-    <hyperlink ref="B77:C77" r:id="rId76"/>
-    <hyperlink ref="B78:C78" r:id="rId77"/>
-    <hyperlink ref="B79:C79" r:id="rId78"/>
-    <hyperlink ref="B80:C80" r:id="rId79"/>
-    <hyperlink ref="B81:C81" r:id="rId80"/>
-    <hyperlink ref="B82:C82" r:id="rId81"/>
-    <hyperlink ref="B83:C83" r:id="rId82"/>
-    <hyperlink ref="B84:C84" r:id="rId83"/>
-    <hyperlink ref="B85:C85" r:id="rId84"/>
-    <hyperlink ref="B86:C86" r:id="rId85"/>
-    <hyperlink ref="B87:C87" r:id="rId86"/>
-    <hyperlink ref="B88:C88" r:id="rId87"/>
-    <hyperlink ref="B89:C89" r:id="rId88"/>
-    <hyperlink ref="B90:C90" r:id="rId89"/>
-    <hyperlink ref="B91:C91" r:id="rId90"/>
-    <hyperlink ref="B92:C92" r:id="rId91"/>
-    <hyperlink ref="B93:C93" r:id="rId92"/>
-    <hyperlink ref="B94:C94" r:id="rId93"/>
-    <hyperlink ref="B95:C95" r:id="rId94"/>
-    <hyperlink ref="B96:C96" r:id="rId95"/>
-    <hyperlink ref="B97:C97" r:id="rId96"/>
-    <hyperlink ref="B98:C98" r:id="rId97"/>
-    <hyperlink ref="B99:C99" r:id="rId98"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="C6" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="C7" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="C8" r:id="rId1"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="C9" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="C10" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="C11" r:id="rId2"/>
+    <hyperlink ref="B12" r:id="rId11"/>
+    <hyperlink ref="C12" r:id="rId1"/>
+    <hyperlink ref="B13" r:id="rId12"/>
+    <hyperlink ref="C13" r:id="rId2"/>
+    <hyperlink ref="B14" r:id="rId13"/>
+    <hyperlink ref="C14" r:id="rId1"/>
+    <hyperlink ref="B15" r:id="rId14"/>
+    <hyperlink ref="C15" r:id="rId2"/>
+    <hyperlink ref="B16" r:id="rId15"/>
+    <hyperlink ref="C16" r:id="rId1"/>
+    <hyperlink ref="B17" r:id="rId16"/>
+    <hyperlink ref="C17" r:id="rId2"/>
+    <hyperlink ref="B18" r:id="rId17"/>
+    <hyperlink ref="C18" r:id="rId1"/>
+    <hyperlink ref="B19" r:id="rId18"/>
+    <hyperlink ref="C19" r:id="rId2"/>
+    <hyperlink ref="B20" r:id="rId19"/>
+    <hyperlink ref="C20" r:id="rId1"/>
+    <hyperlink ref="B21" r:id="rId20"/>
+    <hyperlink ref="C21" r:id="rId2"/>
+    <hyperlink ref="B22" r:id="rId21"/>
+    <hyperlink ref="C22" r:id="rId1"/>
+    <hyperlink ref="B23" r:id="rId22"/>
+    <hyperlink ref="C23" r:id="rId2"/>
+    <hyperlink ref="B24" r:id="rId23"/>
+    <hyperlink ref="C24" r:id="rId1"/>
+    <hyperlink ref="B25" r:id="rId24"/>
+    <hyperlink ref="C25" r:id="rId2"/>
+    <hyperlink ref="B26" r:id="rId25"/>
+    <hyperlink ref="C26" r:id="rId1"/>
+    <hyperlink ref="B27" r:id="rId26"/>
+    <hyperlink ref="C27" r:id="rId2"/>
+    <hyperlink ref="B28" r:id="rId27"/>
+    <hyperlink ref="C28" r:id="rId1"/>
+    <hyperlink ref="B29" r:id="rId28"/>
+    <hyperlink ref="C29" r:id="rId2"/>
+    <hyperlink ref="B30" r:id="rId29"/>
+    <hyperlink ref="C30" r:id="rId1"/>
+    <hyperlink ref="B31" r:id="rId30"/>
+    <hyperlink ref="C31" r:id="rId2"/>
+    <hyperlink ref="B32" r:id="rId31"/>
+    <hyperlink ref="C32" r:id="rId1"/>
+    <hyperlink ref="B33" r:id="rId32"/>
+    <hyperlink ref="C33" r:id="rId2"/>
+    <hyperlink ref="B34" r:id="rId33"/>
+    <hyperlink ref="C34" r:id="rId1"/>
+    <hyperlink ref="B35" r:id="rId34"/>
+    <hyperlink ref="C35" r:id="rId2"/>
+    <hyperlink ref="B36" r:id="rId35"/>
+    <hyperlink ref="C36" r:id="rId1"/>
+    <hyperlink ref="B37" r:id="rId36"/>
+    <hyperlink ref="C37" r:id="rId2"/>
+    <hyperlink ref="B38" r:id="rId37"/>
+    <hyperlink ref="C38" r:id="rId1"/>
+    <hyperlink ref="B39" r:id="rId38"/>
+    <hyperlink ref="C39" r:id="rId2"/>
+    <hyperlink ref="B40" r:id="rId39"/>
+    <hyperlink ref="C40" r:id="rId1"/>
+    <hyperlink ref="B41" r:id="rId40"/>
+    <hyperlink ref="C41" r:id="rId2"/>
+    <hyperlink ref="B42" r:id="rId41"/>
+    <hyperlink ref="C42" r:id="rId1"/>
+    <hyperlink ref="B43" r:id="rId42"/>
+    <hyperlink ref="C43" r:id="rId2"/>
+    <hyperlink ref="B44" r:id="rId43"/>
+    <hyperlink ref="C44" r:id="rId1"/>
+    <hyperlink ref="B45" r:id="rId44"/>
+    <hyperlink ref="C45" r:id="rId2"/>
+    <hyperlink ref="B46" r:id="rId45"/>
+    <hyperlink ref="C46" r:id="rId1"/>
+    <hyperlink ref="B47" r:id="rId46"/>
+    <hyperlink ref="C47" r:id="rId2"/>
+    <hyperlink ref="B48" r:id="rId47"/>
+    <hyperlink ref="C48" r:id="rId1"/>
+    <hyperlink ref="B49" r:id="rId48"/>
+    <hyperlink ref="C49" r:id="rId2"/>
+    <hyperlink ref="B50" r:id="rId49"/>
+    <hyperlink ref="C50" r:id="rId1"/>
+    <hyperlink ref="B51" r:id="rId50"/>
+    <hyperlink ref="C51" r:id="rId2"/>
+    <hyperlink ref="B52" r:id="rId51"/>
+    <hyperlink ref="C52" r:id="rId1"/>
+    <hyperlink ref="B53" r:id="rId52"/>
+    <hyperlink ref="C53" r:id="rId2"/>
+    <hyperlink ref="B54" r:id="rId53"/>
+    <hyperlink ref="C54" r:id="rId1"/>
+    <hyperlink ref="B55" r:id="rId54"/>
+    <hyperlink ref="C55" r:id="rId2"/>
+    <hyperlink ref="B56" r:id="rId55"/>
+    <hyperlink ref="C56" r:id="rId1"/>
+    <hyperlink ref="B57" r:id="rId56"/>
+    <hyperlink ref="C57" r:id="rId2"/>
+    <hyperlink ref="B58" r:id="rId57"/>
+    <hyperlink ref="C58" r:id="rId1"/>
+    <hyperlink ref="B59" r:id="rId58"/>
+    <hyperlink ref="C59" r:id="rId1"/>
+    <hyperlink ref="B60" r:id="rId59"/>
+    <hyperlink ref="C60" r:id="rId2"/>
+    <hyperlink ref="B61" r:id="rId60"/>
+    <hyperlink ref="C61" r:id="rId1"/>
+    <hyperlink ref="B62" r:id="rId61"/>
+    <hyperlink ref="C62" r:id="rId2"/>
+    <hyperlink ref="B63" r:id="rId62"/>
+    <hyperlink ref="C63" r:id="rId1"/>
+    <hyperlink ref="B64" r:id="rId63"/>
+    <hyperlink ref="C64" r:id="rId2"/>
+    <hyperlink ref="B65" r:id="rId64"/>
+    <hyperlink ref="C65" r:id="rId1"/>
+    <hyperlink ref="B66" r:id="rId65"/>
+    <hyperlink ref="C66" r:id="rId2"/>
+    <hyperlink ref="B67" r:id="rId66"/>
+    <hyperlink ref="C67" r:id="rId1"/>
+    <hyperlink ref="B68" r:id="rId67"/>
+    <hyperlink ref="C68" r:id="rId2"/>
+    <hyperlink ref="B69" r:id="rId68"/>
+    <hyperlink ref="C69" r:id="rId1"/>
+    <hyperlink ref="B70" r:id="rId69"/>
+    <hyperlink ref="C70" r:id="rId2"/>
+    <hyperlink ref="B71" r:id="rId70"/>
+    <hyperlink ref="C71" r:id="rId1"/>
+    <hyperlink ref="B72" r:id="rId71"/>
+    <hyperlink ref="C72" r:id="rId2"/>
+    <hyperlink ref="B73" r:id="rId72"/>
+    <hyperlink ref="C73" r:id="rId1"/>
+    <hyperlink ref="B74" r:id="rId73"/>
+    <hyperlink ref="C74" r:id="rId2"/>
+    <hyperlink ref="B75" r:id="rId74"/>
+    <hyperlink ref="C75" r:id="rId1"/>
+    <hyperlink ref="B76" r:id="rId75"/>
+    <hyperlink ref="C76" r:id="rId2"/>
+    <hyperlink ref="B77" r:id="rId76"/>
+    <hyperlink ref="C77" r:id="rId1"/>
+    <hyperlink ref="B78" r:id="rId77"/>
+    <hyperlink ref="C78" r:id="rId2"/>
+    <hyperlink ref="B79" r:id="rId78"/>
+    <hyperlink ref="C79" r:id="rId1"/>
+    <hyperlink ref="B80" r:id="rId79"/>
+    <hyperlink ref="C80" r:id="rId1"/>
+    <hyperlink ref="B81" r:id="rId80"/>
+    <hyperlink ref="C81" r:id="rId2"/>
+    <hyperlink ref="B82" r:id="rId81"/>
+    <hyperlink ref="C82" r:id="rId1"/>
+    <hyperlink ref="B83" r:id="rId82"/>
+    <hyperlink ref="C83" r:id="rId2"/>
+    <hyperlink ref="B84" r:id="rId83"/>
+    <hyperlink ref="C84" r:id="rId1"/>
+    <hyperlink ref="B85" r:id="rId84"/>
+    <hyperlink ref="C85" r:id="rId2"/>
+    <hyperlink ref="B86" r:id="rId85"/>
+    <hyperlink ref="C86" r:id="rId1"/>
+    <hyperlink ref="B87" r:id="rId86"/>
+    <hyperlink ref="C87" r:id="rId2"/>
+    <hyperlink ref="B88" r:id="rId87"/>
+    <hyperlink ref="C88" r:id="rId1"/>
+    <hyperlink ref="B89" r:id="rId88"/>
+    <hyperlink ref="C89" r:id="rId2"/>
+    <hyperlink ref="B90" r:id="rId89"/>
+    <hyperlink ref="C90" r:id="rId1"/>
+    <hyperlink ref="B91" r:id="rId90"/>
+    <hyperlink ref="C91" r:id="rId2"/>
+    <hyperlink ref="B92" r:id="rId91"/>
+    <hyperlink ref="C92" r:id="rId1"/>
+    <hyperlink ref="B93" r:id="rId92"/>
+    <hyperlink ref="C93" r:id="rId2"/>
+    <hyperlink ref="B94" r:id="rId93"/>
+    <hyperlink ref="C94" r:id="rId1"/>
+    <hyperlink ref="B95" r:id="rId94"/>
+    <hyperlink ref="C95" r:id="rId1"/>
+    <hyperlink ref="B96" r:id="rId95"/>
+    <hyperlink ref="C96" r:id="rId2"/>
+    <hyperlink ref="B97" r:id="rId96"/>
+    <hyperlink ref="C97" r:id="rId1"/>
+    <hyperlink ref="B98" r:id="rId97"/>
+    <hyperlink ref="C98" r:id="rId2"/>
+    <hyperlink ref="B99" r:id="rId98"/>
+    <hyperlink ref="C99" r:id="rId1"/>
   </hyperlinks>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1645282330" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1646179446" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -5315,14 +5783,71 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1645282330" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1645282330" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1646179446" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1646179446" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1645282330" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1646179446" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView view="normal" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
+  <cols>
+    <col min="1" max="1" width="38.360360" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1646179446" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="1.000000" right="1.000000" top="1.000000" bottom="1.000000" header="0.393750" footer="0.393750"/>
+  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1646179446" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1646179446" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1646179446" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>